<commit_message>
chore_feat_fix: Reorganiza carpetas, Agrega un script de la Unet normal y Corrige errores de archivos grandes
Se agrega el script de Unet_MICCAI_DS_pytorch y se agrega la carpeta de los modelos al gitignore.
</commit_message>
<xml_diff>
--- a/SegmentationNetworks/trained_Models/Datos de los modelos.xlsx
+++ b/SegmentationNetworks/trained_Models/Datos de los modelos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5711c7b7e65f298f/Documents/DFU_Proyect/SegmentationNetworks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\am969\Documents\DFU_Proyect\SegmentationNetworks\trained_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="8_{1CC92A0F-88DE-426D-8F42-6E1ABCEC37C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB38D5B2-15EF-46F2-8986-CFDCCD16DBE9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836E0F6-0F1B-46B6-8B10-AFD4F4932694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD392E40-C48D-4EA3-9641-62335EC571EC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="72">
   <si>
     <t>Modelo</t>
   </si>
@@ -216,6 +216,42 @@
   </si>
   <si>
     <t>1:30h</t>
+  </si>
+  <si>
+    <t>Acc_val_best</t>
+  </si>
+  <si>
+    <t>Dice_val_best</t>
+  </si>
+  <si>
+    <t>New:</t>
+  </si>
+  <si>
+    <t>ReduceLROnPlateau</t>
+  </si>
+  <si>
+    <t>patience (sched)</t>
+  </si>
+  <si>
+    <t>Colab</t>
+  </si>
+  <si>
+    <t>UnetPytorch_MICCAI_DS.ipynb</t>
+  </si>
+  <si>
+    <t>cuenta</t>
+  </si>
+  <si>
+    <t>am96929</t>
+  </si>
+  <si>
+    <t>LR_scheduling</t>
+  </si>
+  <si>
+    <t>45 min (aprox.)</t>
+  </si>
+  <si>
+    <t>ResUnet_MICCAI_DS.ipynb</t>
   </si>
 </sst>
 </file>
@@ -242,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +339,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -316,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -333,6 +387,13 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,10 +424,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -687,10 +744,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094303F8-B3BE-4038-9DA7-345129856998}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AE35"/>
+  <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,44 +767,44 @@
     <col min="26" max="26" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="S1" s="15" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="S1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
       <c r="Y1" s="9"/>
-      <c r="AA1" s="14" t="s">
+      <c r="AA1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -834,7 +891,7 @@
       </c>
       <c r="AE2" s="5"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -914,7 +971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -945,7 +1002,7 @@
       <c r="J4" t="s">
         <v>36</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="18">
         <v>99.74</v>
       </c>
       <c r="L4" s="2">
@@ -991,7 +1048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1068,7 +1125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1146,7 +1203,7 @@
       </c>
       <c r="AD6" s="7"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1180,7 +1237,7 @@
       <c r="K7" s="8">
         <v>99.53</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="17">
         <v>0.89300000000000002</v>
       </c>
       <c r="M7" s="2">
@@ -1223,7 +1280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1300,7 +1357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1381,77 +1438,344 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="N10" s="12"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="N12" s="12"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="J13" s="7"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH12" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI12" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>45637</v>
+      </c>
+      <c r="F13">
+        <v>1010</v>
+      </c>
+      <c r="G13">
+        <v>808</v>
+      </c>
+      <c r="H13">
+        <v>101</v>
+      </c>
+      <c r="I13">
+        <v>101</v>
+      </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="19">
+        <f>0.9971*100</f>
+        <v>99.71</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0.91310000000000002</v>
+      </c>
+      <c r="M13" s="13">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0.80530000000000002</v>
+      </c>
+      <c r="O13" t="s">
+        <v>70</v>
+      </c>
+      <c r="P13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>25</v>
+      </c>
+      <c r="S13">
+        <v>110</v>
+      </c>
+      <c r="T13" s="3">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="U13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V13" t="s">
+        <v>43</v>
+      </c>
+      <c r="W13">
+        <v>16</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF13">
+        <v>5</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45638</v>
+      </c>
+      <c r="F14">
+        <v>1010</v>
+      </c>
+      <c r="G14">
+        <v>808</v>
+      </c>
+      <c r="H14">
+        <v>101</v>
+      </c>
+      <c r="I14">
+        <v>101</v>
+      </c>
+      <c r="J14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14">
+        <f>0.9972*100</f>
+        <v>99.72</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.89419999999999999</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.99650000000000005</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0.77659999999999996</v>
+      </c>
+      <c r="O14" s="20">
+        <v>6.25E-2</v>
+      </c>
+      <c r="P14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S14">
+        <v>110</v>
+      </c>
+      <c r="T14" s="3">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="U14" t="s">
+        <v>20</v>
+      </c>
+      <c r="V14" t="s">
+        <v>43</v>
+      </c>
+      <c r="W14">
+        <v>16</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB14">
+        <v>2</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF14">
+        <v>5</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:35" x14ac:dyDescent="0.3">
+      <c r="G17" s="7"/>
       <c r="N17" s="12"/>
-    </row>
-    <row r="18" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="AI17" s="7"/>
+    </row>
+    <row r="18" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N24" s="12"/>
     </row>
-    <row r="25" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N25" s="12"/>
     </row>
-    <row r="26" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N26" s="12"/>
     </row>
-    <row r="27" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N27" s="12"/>
     </row>
-    <row r="28" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N28" s="10"/>
     </row>
-    <row r="29" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N29" s="10"/>
     </row>
-    <row r="30" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N30" s="10"/>
     </row>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N31" s="10"/>
     </row>
-    <row r="32" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:35" x14ac:dyDescent="0.3">
       <c r="N32" s="10"/>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore: actualiza los datos de los modelos entrenados
</commit_message>
<xml_diff>
--- a/SegmentationNetworks/trained_Models/Datos de los modelos.xlsx
+++ b/SegmentationNetworks/trained_Models/Datos de los modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\am969\Documents\DFU_Proyect\SegmentationNetworks\trained_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836E0F6-0F1B-46B6-8B10-AFD4F4932694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27BC8E6-6C6D-4606-A30A-CFA2952E8463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD392E40-C48D-4EA3-9641-62335EC571EC}"/>
   </bookViews>
@@ -370,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -403,6 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,8 +747,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1484,7 +1485,7 @@
       <c r="M12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="24" t="s">
         <v>6</v>
       </c>
       <c r="O12" s="6" t="s">
@@ -1734,6 +1735,7 @@
       <c r="AI17" s="7"/>
     </row>
     <row r="18" spans="7:35" x14ac:dyDescent="0.3">
+      <c r="J18" s="7"/>
       <c r="N18" s="12"/>
     </row>
     <row r="19" spans="7:35" x14ac:dyDescent="0.3">

</xml_diff>